<commit_message>
update constraint & bounds logic
</commit_message>
<xml_diff>
--- a/data/plan_inputs/bounds.xlsx
+++ b/data/plan_inputs/bounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\plan_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8CD2F7-3803-4FC0-8315-821D92049EF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D7AB35-E858-48F4-90D3-93B9074B7EDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6360" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IBT" sheetId="1" r:id="rId1"/>
@@ -2783,7 +2783,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,7 +2823,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2856,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3087,7 +3087,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3138,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3160,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3171,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update report to have fs adjusted weights
</commit_message>
<xml_diff>
--- a/data/plan_inputs/bounds.xlsx
+++ b/data/plan_inputs/bounds.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\plan_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\plan_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D7AB35-E858-48F4-90D3-93B9074B7EDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F832E1-DB3D-4079-8993-66A781A26788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IBT" sheetId="1" r:id="rId1"/>
     <sheet name="Pension" sheetId="2" r:id="rId2"/>
     <sheet name="Retirement" sheetId="3" r:id="rId3"/>
+    <sheet name="Unbounded" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="Covariance">'[1]Covariance Matrix'!$G$7:$Z$26</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>Asset/Liability</t>
   </si>
@@ -2783,17 +2784,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2815,7 +2816,7 @@
         <v>-0.99999999999999001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2826,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2848,73 +2849,73 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C8" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C9" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C10" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C11" s="2">
-        <v>1.00000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.00000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2935,17 +2936,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2956,7 +2957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>-0.99999999999999001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2978,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2989,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3000,73 +3001,73 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C8" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="C9" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="C10" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C11" s="2">
-        <v>1.00000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.00000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -3087,17 +3088,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3108,7 +3109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3119,7 +3120,7 @@
         <v>-0.99999999999999001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3130,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3152,18 +3153,170 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
+        <v>0.15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.02</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0.02</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.02</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.00000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82264CC-04BC-4320-B90A-7328F405EEC2}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-1.0000000000010001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-0.99999999999999001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3174,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3182,10 +3335,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3193,10 +3346,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3204,10 +3357,10 @@
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3215,10 +3368,10 @@
         <v>0.01</v>
       </c>
       <c r="C11" s="2">
-        <v>1.00000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.00000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>

</xml_diff>